<commit_message>
Evaluation result has a chart displayed now
</commit_message>
<xml_diff>
--- a/tests/ragas_evaluation_results.xlsx
+++ b/tests/ragas_evaluation_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="630" yWindow="540" windowWidth="27495" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -12,13 +12,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="112">
   <si>
     <t>user_input</t>
   </si>
@@ -507,9 +507,6 @@
   </si>
   <si>
     <t>Row Labels</t>
-  </si>
-  <si>
-    <t>(blank)</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -591,6 +588,427 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[ragas_evaluation_results.xlsx]Summary!PivotTable1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average of faithfulness</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Multi-Context</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Reasoning</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Simple</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.98275862068965525</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94416100705407668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9732804232804233</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average of answer_relevancy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Multi-Context</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Reasoning</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Simple</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.89687672979207222</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89230532336756185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83588268393877929</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average of context_precision</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Multi-Context</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Reasoning</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Simple</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.49999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57142857137142855</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.85714285705714288</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average of context_recall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Multi-Context</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Reasoning</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Simple</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$E$4:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35714285714285715</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summary!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average of context_entity_recall</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summary!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Multi-Context</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Reasoning</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Simple</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summary!$F$4:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.19999999960000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19523809468492062</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38333333168769845</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="224405760"/>
+        <c:axId val="225049600"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="224405760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="225049600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="225049600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="224405760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -937,8 +1355,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:F8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+  <location ref="A3:F7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -949,12 +1367,12 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" multipleItemSelectionAllowed="1" showAll="0">
       <items count="5">
         <item x="2"/>
         <item x="1"/>
         <item x="0"/>
-        <item x="3"/>
+        <item h="1" x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -962,7 +1380,7 @@
   <rowFields count="1">
     <field x="9"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="4">
     <i>
       <x/>
     </i>
@@ -971,9 +1389,6 @@
     </i>
     <i>
       <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
     </i>
     <i t="grand">
       <x/>
@@ -1006,6 +1421,53 @@
     <dataField name="Average of context_recall" fld="7" subtotal="average" baseField="9" baseItem="3" numFmtId="2"/>
     <dataField name="Average of context_entity_recall" fld="8" subtotal="average" baseField="9" baseItem="3" numFmtId="2"/>
   </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -1300,18 +1762,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F8"/>
+  <dimension ref="A3:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1400,35 +1862,26 @@
       <c r="A7" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B8" s="5">
+      <c r="B7" s="5">
         <v>0.96524218333407708</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C7" s="5">
         <v>0.85835862166521681</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D7" s="5">
         <v>0.73913043470869555</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E7" s="5">
         <v>0.42753623188405793</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F7" s="5">
         <v>0.31014492633140095</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1436,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>